<commit_message>
bom updated - pcb library updated
</commit_message>
<xml_diff>
--- a/pcb/wifi_ledstrip/bom.xlsx
+++ b/pcb/wifi_ledstrip/bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\uC\esp8266-stm32f103c8-ws2811\pcb\wifi_ledstrip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27017F6E-819D-4390-BE7C-F243BA146A12}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A587DB9-E4EB-4B28-863A-AFFFA8CCEE1A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16457" windowHeight="6986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16455" windowHeight="6990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bom_2" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="203">
   <si>
     <t>Qty</t>
   </si>
@@ -603,12 +603,57 @@
   </si>
   <si>
     <t>lomex</t>
+  </si>
+  <si>
+    <t>ledek</t>
+  </si>
+  <si>
+    <t>piros</t>
+  </si>
+  <si>
+    <t>sarga</t>
+  </si>
+  <si>
+    <t>kek</t>
+  </si>
+  <si>
+    <t>feher</t>
+  </si>
+  <si>
+    <t>narancs</t>
+  </si>
+  <si>
+    <t>darabszam</t>
+  </si>
+  <si>
+    <t>ellenallasok</t>
+  </si>
+  <si>
+    <t>aram</t>
+  </si>
+  <si>
+    <t>feszultseg</t>
+  </si>
+  <si>
+    <t>ellenallas ledekhez</t>
+  </si>
+  <si>
+    <t>rendelendo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="7">
+    <numFmt numFmtId="164" formatCode="General&quot; db&quot;"/>
+    <numFmt numFmtId="165" formatCode="General&quot; mA&quot;"/>
+    <numFmt numFmtId="166" formatCode="0&quot; V&quot;"/>
+    <numFmt numFmtId="171" formatCode="0.#&quot; V&quot;"/>
+    <numFmt numFmtId="172" formatCode="#,##0&quot; V&quot;"/>
+    <numFmt numFmtId="173" formatCode="General&quot; Ohm&quot;"/>
+    <numFmt numFmtId="174" formatCode="#,###&quot; V&quot;"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1086,9 +1131,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1444,28 +1499,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.15234375" customWidth="1"/>
-    <col min="2" max="2" width="14.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16.3828125" customWidth="1"/>
-    <col min="5" max="5" width="16.15234375" customWidth="1"/>
-    <col min="6" max="6" width="19.3046875" customWidth="1"/>
-    <col min="7" max="7" width="26.69140625" customWidth="1"/>
-    <col min="8" max="8" width="47.765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.765625" customWidth="1"/>
-    <col min="12" max="12" width="9.53515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.15234375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.4609375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="8" max="8" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>86</v>
       </c>
@@ -1503,7 +1558,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -1537,7 +1592,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -1570,7 +1625,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -1603,7 +1658,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>179</v>
       </c>
@@ -1633,7 +1688,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1663,12 +1718,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>179</v>
       </c>
@@ -1698,7 +1753,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>179</v>
       </c>
@@ -1728,7 +1783,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -1758,7 +1813,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>179</v>
       </c>
@@ -1788,7 +1843,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -1818,7 +1873,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -1848,7 +1903,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>187</v>
       </c>
@@ -1878,7 +1933,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>187</v>
       </c>
@@ -1908,7 +1963,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>188</v>
       </c>
@@ -1935,7 +1990,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>179</v>
       </c>
@@ -1959,7 +2014,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -1983,7 +2038,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>87</v>
       </c>
@@ -2007,7 +2062,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -2034,7 +2089,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -2064,7 +2119,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -2094,7 +2149,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>87</v>
       </c>
@@ -2121,7 +2176,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -2145,7 +2200,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -2172,7 +2227,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>87</v>
       </c>
@@ -2196,77 +2251,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>186</v>
-      </c>
-      <c r="B32">
-        <f>C32*4+1</f>
-        <v>33</v>
-      </c>
-      <c r="C32">
-        <v>8</v>
-      </c>
-      <c r="F32" t="s">
-        <v>26</v>
-      </c>
-      <c r="G32" t="s">
-        <v>27</v>
-      </c>
-      <c r="H32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I32" t="s">
-        <v>29</v>
-      </c>
-      <c r="M32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
-        <v>189</v>
-      </c>
-      <c r="B33">
-        <f>C33*4+1</f>
-        <v>33</v>
-      </c>
-      <c r="C33">
-        <v>8</v>
-      </c>
-      <c r="E33" t="s">
-        <v>65</v>
-      </c>
-      <c r="F33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G33" t="s">
-        <v>67</v>
-      </c>
-      <c r="H33" t="s">
-        <v>68</v>
-      </c>
-      <c r="I33" t="s">
-        <v>69</v>
-      </c>
-      <c r="J33" t="s">
-        <v>70</v>
-      </c>
-      <c r="N33" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>159</v>
       </c>
@@ -2304,7 +2294,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>147</v>
       </c>
@@ -2342,7 +2332,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>136</v>
       </c>
@@ -2380,7 +2370,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>131</v>
       </c>
@@ -2418,7 +2408,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>127</v>
       </c>
@@ -2438,7 +2428,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>122</v>
       </c>
@@ -2476,7 +2466,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>117</v>
       </c>
@@ -2514,7 +2504,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -2552,7 +2542,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>101</v>
       </c>
@@ -2590,7 +2580,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -2628,12 +2618,12 @@
         <v>805</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>159</v>
       </c>
@@ -2671,7 +2661,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>147</v>
       </c>
@@ -2709,7 +2699,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>136</v>
       </c>
@@ -2747,7 +2737,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>131</v>
       </c>
@@ -2785,7 +2775,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>127</v>
       </c>
@@ -2805,7 +2795,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>122</v>
       </c>
@@ -2843,7 +2833,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>117</v>
       </c>
@@ -2881,7 +2871,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>110</v>
       </c>
@@ -2919,7 +2909,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>101</v>
       </c>
@@ -2957,7 +2947,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>96</v>
       </c>
@@ -2993,6 +2983,317 @@
       </c>
       <c r="M57">
         <v>805</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>186</v>
+      </c>
+      <c r="B62">
+        <f>C62*4+1</f>
+        <v>33</v>
+      </c>
+      <c r="C62">
+        <v>8</v>
+      </c>
+      <c r="F62" t="s">
+        <v>26</v>
+      </c>
+      <c r="G62" t="s">
+        <v>27</v>
+      </c>
+      <c r="H62" t="s">
+        <v>28</v>
+      </c>
+      <c r="I62" t="s">
+        <v>29</v>
+      </c>
+      <c r="M62" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>189</v>
+      </c>
+      <c r="B63">
+        <f>C63*4+1</f>
+        <v>33</v>
+      </c>
+      <c r="C63">
+        <v>8</v>
+      </c>
+      <c r="E63" t="s">
+        <v>65</v>
+      </c>
+      <c r="F63" t="s">
+        <v>66</v>
+      </c>
+      <c r="G63" t="s">
+        <v>67</v>
+      </c>
+      <c r="H63" t="s">
+        <v>68</v>
+      </c>
+      <c r="I63" t="s">
+        <v>69</v>
+      </c>
+      <c r="J63" t="s">
+        <v>70</v>
+      </c>
+      <c r="N63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="B66" t="s">
+        <v>197</v>
+      </c>
+      <c r="C66" t="s">
+        <v>200</v>
+      </c>
+      <c r="D66" t="s">
+        <v>199</v>
+      </c>
+      <c r="E66" s="4">
+        <v>12</v>
+      </c>
+      <c r="F66" s="4">
+        <v>5</v>
+      </c>
+      <c r="G66" s="5">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>192</v>
+      </c>
+      <c r="B67" s="2">
+        <v>10</v>
+      </c>
+      <c r="C67" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="D67" s="3">
+        <v>20</v>
+      </c>
+      <c r="E67" s="7">
+        <f>(E$66-$C67)/$D67*1000</f>
+        <v>495</v>
+      </c>
+      <c r="F67" s="7">
+        <f t="shared" ref="F67:G67" si="1">(F$66-$C67)/$D67*1000</f>
+        <v>145</v>
+      </c>
+      <c r="G67" s="7">
+        <f t="shared" si="1"/>
+        <v>59.999999999999986</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>195</v>
+      </c>
+      <c r="B68" s="2">
+        <v>10</v>
+      </c>
+      <c r="C68" s="6">
+        <v>3</v>
+      </c>
+      <c r="D68" s="3">
+        <v>20</v>
+      </c>
+      <c r="E68" s="7">
+        <f t="shared" ref="E68:G72" si="2">(E$66-$C68)/$D68*1000</f>
+        <v>450</v>
+      </c>
+      <c r="F68" s="7">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="G68" s="7">
+        <f t="shared" si="2"/>
+        <v>14.999999999999991</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>193</v>
+      </c>
+      <c r="B69" s="2">
+        <v>10</v>
+      </c>
+      <c r="C69" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="D69" s="3">
+        <v>20</v>
+      </c>
+      <c r="E69" s="7">
+        <f t="shared" si="2"/>
+        <v>495</v>
+      </c>
+      <c r="F69" s="7">
+        <f t="shared" si="2"/>
+        <v>145</v>
+      </c>
+      <c r="G69" s="7">
+        <f t="shared" si="2"/>
+        <v>59.999999999999986</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>194</v>
+      </c>
+      <c r="B70" s="2">
+        <v>10</v>
+      </c>
+      <c r="C70" s="6">
+        <v>3</v>
+      </c>
+      <c r="D70" s="3">
+        <v>20</v>
+      </c>
+      <c r="E70" s="7">
+        <f t="shared" si="2"/>
+        <v>450</v>
+      </c>
+      <c r="F70" s="7">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="G70" s="7">
+        <f t="shared" si="2"/>
+        <v>14.999999999999991</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>196</v>
+      </c>
+      <c r="B71" s="2">
+        <v>10</v>
+      </c>
+      <c r="C71" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="D71" s="3">
+        <v>20</v>
+      </c>
+      <c r="E71" s="7">
+        <f t="shared" si="2"/>
+        <v>495</v>
+      </c>
+      <c r="F71" s="7">
+        <f t="shared" si="2"/>
+        <v>145</v>
+      </c>
+      <c r="G71" s="7">
+        <f t="shared" si="2"/>
+        <v>59.999999999999986</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C73" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="7">
+        <v>495</v>
+      </c>
+      <c r="B74" s="7">
+        <v>510</v>
+      </c>
+      <c r="C74" s="2">
+        <f>10*3</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="7">
+        <v>450</v>
+      </c>
+      <c r="B75" s="7">
+        <v>470</v>
+      </c>
+      <c r="C75" s="2">
+        <f>10*2</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="7">
+        <v>145</v>
+      </c>
+      <c r="B76" s="7">
+        <v>150</v>
+      </c>
+      <c r="C76" s="2">
+        <f>10*3</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="7">
+        <v>100</v>
+      </c>
+      <c r="B77" s="7">
+        <v>100</v>
+      </c>
+      <c r="C77" s="2">
+        <f>10*2</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="7">
+        <v>60</v>
+      </c>
+      <c r="B78" s="7">
+        <v>62</v>
+      </c>
+      <c r="C78" s="2">
+        <f>10*3</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="7">
+        <v>15</v>
+      </c>
+      <c r="B79" s="7">
+        <v>15</v>
+      </c>
+      <c r="C79" s="2">
+        <f>10*2</f>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3000,6 +3301,7 @@
     <sortCondition ref="M1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3011,20 +3313,20 @@
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.4609375" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="6" max="6" width="15.4609375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.3046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.4609375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.3046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.84375" customWidth="1"/>
-    <col min="11" max="11" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>159</v>
       </c>
@@ -3062,7 +3364,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -3100,7 +3402,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>136</v>
       </c>
@@ -3138,7 +3440,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>131</v>
       </c>
@@ -3176,7 +3478,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -3196,7 +3498,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>122</v>
       </c>
@@ -3234,7 +3536,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -3272,7 +3574,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>110</v>
       </c>
@@ -3310,7 +3612,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -3348,7 +3650,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>96</v>
       </c>
@@ -3399,9 +3701,9 @@
       <selection sqref="A1:L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>159</v>
       </c>
@@ -3439,7 +3741,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -3477,7 +3779,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>136</v>
       </c>
@@ -3515,7 +3817,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>131</v>
       </c>
@@ -3553,7 +3855,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -3573,7 +3875,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>122</v>
       </c>
@@ -3611,7 +3913,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -3649,7 +3951,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>110</v>
       </c>
@@ -3687,7 +3989,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -3725,7 +4027,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>96</v>
       </c>

</xml_diff>